<commit_message>
yet another organisation change
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,19 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="16-20 consecutive" sheetId="2" r:id="rId2"/>
-    <sheet name="17-28 consecutive" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>count = 1000</t>
   </si>
@@ -33,9 +32,6 @@
   </si>
   <si>
     <t>16-20 consecutive</t>
-  </si>
-  <si>
-    <t>17-28 consecutive</t>
   </si>
   <si>
     <t>count</t>
@@ -384,6 +380,1726 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="uk-UA"/>
+              <a:t>Час виконання (сек)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16-20 consecutive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.12000012397766111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92499899864196777</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.988998174667358</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9829995632171631</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.45099925994873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.154999017715451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.730193376541138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.657998085021973</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>77.397874116897583</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.8469722270966</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>139.93980312347409</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>182.07259964942929</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>232.648802280426</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>290.84969162940979</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>359.49581122398382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$5:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$7:$P$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$8:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$9:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$10:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Main!$B$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$B$11:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-DCD2-4C24-87EF-02F4F6A6FAF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="536124400"/>
+        <c:axId val="536122104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="536124400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536122104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="536122104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="536124400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="30"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>790574</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,72 +2515,26 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="18">
-        <f>'17-28 consecutive'!C2</f>
-        <v>0.1239993572235107</v>
-      </c>
-      <c r="C4" s="19">
-        <f>'17-28 consecutive'!C3</f>
-        <v>0.94499921798706055</v>
-      </c>
-      <c r="D4" s="19">
-        <f>'17-28 consecutive'!C4</f>
-        <v>3.0649957656860352</v>
-      </c>
-      <c r="E4" s="19">
-        <f>'17-28 consecutive'!C5</f>
-        <v>7.1960034370422363</v>
-      </c>
-      <c r="F4" s="19">
-        <f>'17-28 consecutive'!C6</f>
-        <v>13.780641555786129</v>
-      </c>
-      <c r="G4" s="19">
-        <f>'17-28 consecutive'!C7</f>
-        <v>23.784998893737789</v>
-      </c>
-      <c r="H4" s="19">
-        <f>'17-28 consecutive'!C8</f>
-        <v>37.374277114868157</v>
-      </c>
-      <c r="I4" s="19">
-        <f>'17-28 consecutive'!C9</f>
-        <v>55.983834266662598</v>
-      </c>
-      <c r="J4" s="19">
-        <f>'17-28 consecutive'!C10</f>
-        <v>79.177190065383911</v>
-      </c>
-      <c r="K4" s="19">
-        <f>'17-28 consecutive'!C11</f>
-        <v>108.31294727325439</v>
-      </c>
-      <c r="L4" s="19">
-        <f>'17-28 consecutive'!C12</f>
-        <v>143.99176144599909</v>
-      </c>
-      <c r="M4" s="19">
-        <f>'17-28 consecutive'!C13</f>
-        <v>187.02585315704351</v>
-      </c>
-      <c r="N4" s="19">
-        <f>'17-28 consecutive'!C14</f>
-        <v>239.7780034542084</v>
-      </c>
-      <c r="O4" s="19">
-        <f>'17-28 consecutive'!C15</f>
-        <v>299.60829448699951</v>
-      </c>
-      <c r="P4" s="20">
-        <f>'17-28 consecutive'!C16</f>
-        <v>369.73739051818848</v>
-      </c>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="20"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
+      <c r="B5"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -991,6 +2661,7 @@
     <mergeCell ref="B1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -998,28 +2669,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1294,313 +2975,6 @@
       <c r="E16">
         <f t="shared" si="0"/>
         <v>2.7816735794369247</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1000</v>
-      </c>
-      <c r="C2">
-        <v>0.1239993572235107</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E16" si="0">B2/C2</f>
-        <v>8064.5579331309355</v>
-      </c>
-      <c r="G2">
-        <f>SUM(C2:C16)/60</f>
-        <v>26.164753166834512</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>1000</v>
-      </c>
-      <c r="C3">
-        <v>0.94499921798706055</v>
-      </c>
-      <c r="D3">
-        <v>0.02</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>1058.2019338916452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>3.0649957656860352</v>
-      </c>
-      <c r="D4">
-        <v>0.05</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>326.26472479846018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5">
-        <v>7.1960034370422363</v>
-      </c>
-      <c r="D5">
-        <v>0.12</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>138.96602589881874</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>13.780641555786129</v>
-      </c>
-      <c r="D6">
-        <v>0.23</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>72.565562056878719</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>60</v>
-      </c>
-      <c r="B7">
-        <v>1000</v>
-      </c>
-      <c r="C7">
-        <v>23.784998893737789</v>
-      </c>
-      <c r="D7">
-        <v>0.4</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>42.043306559214685</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>70</v>
-      </c>
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
-        <v>37.374277114868157</v>
-      </c>
-      <c r="D8">
-        <v>0.62</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>26.756370348690492</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>80</v>
-      </c>
-      <c r="B9">
-        <v>1000</v>
-      </c>
-      <c r="C9">
-        <v>55.983834266662598</v>
-      </c>
-      <c r="D9">
-        <v>0.93</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>17.862299235111209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>90</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>79.177190065383911</v>
-      </c>
-      <c r="D10">
-        <v>1.32</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>12.629900090849494</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>100</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11">
-        <v>108.31294727325439</v>
-      </c>
-      <c r="D11">
-        <v>1.81</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>9.2325065947764955</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>110</v>
-      </c>
-      <c r="B12">
-        <v>1000</v>
-      </c>
-      <c r="C12">
-        <v>143.99176144599909</v>
-      </c>
-      <c r="D12">
-        <v>2.4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>6.9448417739859911</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>120</v>
-      </c>
-      <c r="B13">
-        <v>1000</v>
-      </c>
-      <c r="C13">
-        <v>187.02585315704351</v>
-      </c>
-      <c r="D13">
-        <v>3.12</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>5.3468543686327212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>130</v>
-      </c>
-      <c r="B14">
-        <v>1000</v>
-      </c>
-      <c r="C14">
-        <v>239.7780034542084</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>4.1705243416582833</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>140</v>
-      </c>
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15">
-        <v>299.60829448699951</v>
-      </c>
-      <c r="D15">
-        <v>4.99</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>3.3376913069520899</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>150</v>
-      </c>
-      <c r="B16">
-        <v>1000</v>
-      </c>
-      <c r="C16">
-        <v>369.73739051818848</v>
-      </c>
-      <c r="D16">
-        <v>6.16</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>2.7046223228829951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shit, i found something worse than kubernetes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -10,6 +10,8 @@
     <sheet name="16-20 consecutive" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="00-35 synchronous" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="14-25 &lt;class 'type'&gt;" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="22-09 synchronous" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="22-33 multiprocessed" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -1356,7 +1358,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1420,7 +1422,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1460,7 +1462,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -2018,12 +2020,31 @@
       <c r="P5" s="4" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="n"/>
-      <c r="B6" s="18" t="n"/>
-      <c r="C6" s="19" t="n"/>
-      <c r="D6" s="19" t="n"/>
-      <c r="E6" s="19" t="n"/>
-      <c r="F6" s="19" t="n"/>
+      <c r="A6" s="17" t="inlineStr">
+        <is>
+          <t>22-09 synchronous</t>
+        </is>
+      </c>
+      <c r="B6" s="18">
+        <f>'22-09 synchronous'!C2</f>
+        <v/>
+      </c>
+      <c r="C6" s="19">
+        <f>'22-09 synchronous'!C3</f>
+        <v/>
+      </c>
+      <c r="D6" s="19">
+        <f>'22-09 synchronous'!C4</f>
+        <v/>
+      </c>
+      <c r="E6" s="19">
+        <f>'22-09 synchronous'!C5</f>
+        <v/>
+      </c>
+      <c r="F6" s="19">
+        <f>'22-09 synchronous'!C6</f>
+        <v/>
+      </c>
       <c r="G6" s="19" t="n"/>
       <c r="H6" s="19" t="n"/>
       <c r="I6" s="19" t="n"/>
@@ -2036,11 +2057,31 @@
       <c r="P6" s="20" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="n"/>
-      <c r="C7" s="11" t="n"/>
-      <c r="D7" s="11" t="n"/>
-      <c r="E7" s="11" t="n"/>
-      <c r="F7" s="11" t="n"/>
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>22-33 multiprocessed</t>
+        </is>
+      </c>
+      <c r="B7">
+        <f>'22-33 multiprocessed'!C2</f>
+        <v/>
+      </c>
+      <c r="C7" s="11">
+        <f>'22-33 multiprocessed'!C3</f>
+        <v/>
+      </c>
+      <c r="D7" s="11">
+        <f>'22-33 multiprocessed'!C4</f>
+        <v/>
+      </c>
+      <c r="E7" s="11">
+        <f>'22-33 multiprocessed'!C5</f>
+        <v/>
+      </c>
+      <c r="F7" s="11">
+        <f>'22-33 multiprocessed'!C6</f>
+        <v/>
+      </c>
       <c r="G7" s="11" t="n"/>
       <c r="H7" s="11" t="n"/>
       <c r="I7" s="11" t="n"/>
@@ -2753,4 +2794,294 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dim</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>time, sec</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>time, min</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>avg matrix/min</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total time spent, min</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>500</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13.18888280000101</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="E2">
+        <f>60*B2/C2</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>SUM(C2:C6)/60</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>750</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>44.4267636999939</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="E3">
+        <f>60*B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>105.522699000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="E4">
+        <f>60*B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>204.777259800001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="E5">
+        <f>60*B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>356.9483743000019</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="E6">
+        <f>60*B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dim</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>time, sec</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>time, min</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>avg matrix/min</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total time spent, min</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>500</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>24.22294069999771</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E2">
+        <f>60*B2/C2</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>SUM(C2:C6)/60</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>750</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>84.81191759999638</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="E3">
+        <f>60*B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>194.1295083000005</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="E4">
+        <f>60*B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>423.212571600001</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7.05</v>
+      </c>
+      <c r="E5">
+        <f>60*B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>695.4124376999971</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11.59</v>
+      </c>
+      <c r="E6">
+        <f>60*B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
i was right all along! how could that be!
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,6 +12,8 @@
     <sheet name="14-25 &lt;class 'type'&gt;" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="22-09 synchronous" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="22-33 multiprocessed" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="00-22 synchronous" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="00-30 multiprocessed" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -2094,12 +2096,31 @@
       <c r="P7" s="4" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="n"/>
-      <c r="B8" s="18" t="n"/>
-      <c r="C8" s="19" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="19" t="n"/>
-      <c r="F8" s="19" t="n"/>
+      <c r="A8" s="17" t="inlineStr">
+        <is>
+          <t>00-22 synchronous</t>
+        </is>
+      </c>
+      <c r="B8" s="18">
+        <f>'00-22 synchronous'!C2</f>
+        <v/>
+      </c>
+      <c r="C8" s="19">
+        <f>'00-22 synchronous'!C3</f>
+        <v/>
+      </c>
+      <c r="D8" s="19">
+        <f>'00-22 synchronous'!C4</f>
+        <v/>
+      </c>
+      <c r="E8" s="19">
+        <f>'00-22 synchronous'!C5</f>
+        <v/>
+      </c>
+      <c r="F8" s="19">
+        <f>'00-22 synchronous'!C6</f>
+        <v/>
+      </c>
       <c r="G8" s="19" t="n"/>
       <c r="H8" s="19" t="n"/>
       <c r="I8" s="19" t="n"/>
@@ -2112,11 +2133,31 @@
       <c r="P8" s="20" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="n"/>
-      <c r="C9" s="11" t="n"/>
-      <c r="D9" s="11" t="n"/>
-      <c r="E9" s="11" t="n"/>
-      <c r="F9" s="11" t="n"/>
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>00-30 multiprocessed</t>
+        </is>
+      </c>
+      <c r="B9">
+        <f>'00-30 multiprocessed'!C2</f>
+        <v/>
+      </c>
+      <c r="C9" s="11">
+        <f>'00-30 multiprocessed'!C3</f>
+        <v/>
+      </c>
+      <c r="D9" s="11">
+        <f>'00-30 multiprocessed'!C4</f>
+        <v/>
+      </c>
+      <c r="E9" s="11">
+        <f>'00-30 multiprocessed'!C5</f>
+        <v/>
+      </c>
+      <c r="F9" s="11">
+        <f>'00-30 multiprocessed'!C6</f>
+        <v/>
+      </c>
       <c r="G9" s="11" t="n"/>
       <c r="H9" s="11" t="n"/>
       <c r="I9" s="11" t="n"/>
@@ -3084,4 +3125,294 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dim</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>time, sec</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>time, min</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>avg matrix/min</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total time spent, min</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1970628000271972</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>60*B2/C2</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>SUM(C2:C6)/60</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>50</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.068523800000548</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E3">
+        <f>60*B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>29.42184979998274</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E4">
+        <f>60*B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>455.9260137999954</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="E5">
+        <f>60*B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>300</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2334.644614599994</v>
+      </c>
+      <c r="D6" t="n">
+        <v>38.91</v>
+      </c>
+      <c r="E6">
+        <f>60*B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dim</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>time, sec</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>time, min</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>avg matrix/min</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total time spent, min</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.78727249999065</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E2">
+        <f>60*B2/C2</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>SUM(C2:C6)/60</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>50</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.066149300022516</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E3">
+        <f>60*B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5.765522300003795</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <f>60*B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>64.40812609999557</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="E5">
+        <f>60*B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>300</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>390.2966042000044</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E6">
+        <f>60*B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>